<commit_message>
Se actualiza inventario excel bd
</commit_message>
<xml_diff>
--- a/BD/BD.xlsx
+++ b/BD/BD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Phoenix/Cursos/mintic/UdeA/cursos/ciclo3/programacion3/proyectos/BD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89C71C2-C15B-AD4F-BE2C-9B1D0A19464E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E6AE52-4161-6345-999A-1EEF97B17E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" activeTab="7" xr2:uid="{5184B347-575A-3747-8A39-CB6109220D64}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" activeTab="6" xr2:uid="{5184B347-575A-3747-8A39-CB6109220D64}"/>
   </bookViews>
   <sheets>
     <sheet name="producto" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="64">
   <si>
     <t>NOT NULL</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>nombre del usuario</t>
+  </si>
+  <si>
+    <t>apellido del usuario</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB9EA59-1F25-7243-855B-925DF68D4DC5}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1256,37 +1262,65 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1299,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F319E60D-9197-EC4B-9C22-DCB7BF938BD1}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>